<commit_message>
added the drive wheel spacer
</commit_message>
<xml_diff>
--- a/bom/exported/rccar-bom-v1.xlsx
+++ b/bom/exported/rccar-bom-v1.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Material" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="111">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -73,7 +74,7 @@
     <t xml:space="preserve">#61 rubber band</t>
   </si>
   <si>
-    <t xml:space="preserve">Alliance Rubber 54615 Advantage Rubber Bands Size #61, 1 lb Box Contains Approx. 535 Bands (2" x 1/4", Blue)</t>
+    <t xml:space="preserve">Alliance Rubber 54615 Advantage Rubber Bands Size #61, 1 lb Box Contains Approx. 535 Bands (2inch x 1/4inch, Blue)</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.com/dp/B008X09UNC</t>
@@ -281,6 +282,78 @@
   </si>
   <si>
     <t xml:space="preserve">only really need the flat one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cura time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material (grams)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel (meters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rcchassis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3hr15min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">servocap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rubberbandwheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3hr7min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motorclip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electronicsriser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2hrs13min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figuring the total time in friendly units:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">axleouterspacer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total time (fract)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractional hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
   </si>
 </sst>
 </file>
@@ -367,7 +440,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,10 +450,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -407,13 +476,14 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,7 +841,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>43</v>
@@ -794,7 +864,7 @@
       </c>
       <c r="H14" s="2" t="n">
         <f aca="false">G14*A14</f>
-        <v>0.277425</v>
+        <v>0.88776</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +1043,7 @@
       <c r="A22" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C22" s="0" t="s">
@@ -997,23 +1067,23 @@
         <v>0.581666666666667</v>
       </c>
     </row>
-    <row r="23" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>6.99</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="0" t="n">
         <v>25</v>
       </c>
       <c r="G23" s="2" t="n">
@@ -1026,7 +1096,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>70</v>
       </c>
       <c r="E25" s="2" t="n">
@@ -1035,7 +1105,7 @@
       </c>
       <c r="H25" s="2" t="n">
         <f aca="false">SUM(H2:H23)</f>
-        <v>20.9058140876725</v>
+        <v>21.5161490876725</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,19 +1116,19 @@
       <c r="A27" s="0" t="n">
         <v>-1</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="0" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>28.99</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G27" s="2" t="n">
@@ -1107,12 +1177,12 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H30" s="2" t="n">
         <f aca="false">SUM(H2:H23)+SUM(H27:H28)</f>
-        <v>19.9058140876725</v>
+        <v>20.5161490876725</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,11 +1293,243 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.19"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">3*60+15</f>
+        <v>195</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">3*60+7</f>
+        <v>187</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">2*60+13</f>
+        <v>133</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="3" t="n">
+        <f aca="false">D9/60</f>
+        <v>9.35</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(H8)</f>
+        <v>9</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <f aca="false">H8-I8</f>
+        <v>0.35</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <f aca="false">ROUND(J8*60,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(I8,"hrs", K8, "min")</f>
+        <v>9hrs21min</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">SUM(D2:D7)</f>
+        <v>561</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">SUM(E2:E6)</f>
+        <v>48</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">SUM(F2:F6)</f>
+        <v>16.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the spacer to the BOM
</commit_message>
<xml_diff>
--- a/bom/exported/rccar-bom-v1.xlsx
+++ b/bom/exported/rccar-bom-v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="114">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -47,6 +47,69 @@
     <t xml:space="preserve">Quantity Needed Price</t>
   </si>
   <si>
+    <t xml:space="preserve">small breadboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEYUE breadboard Set Prototype Board - 6 PCS 400 Pin Solderless Board Kit for Raspberry pi and Arduino Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07LFD4LT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#61 rubber band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alliance Rubber 54615 Advantage Rubber Bands Size #61, 1 lb Box Contains Approx. 535 Bands (2inch x 1/4inch, Blue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B008X09UNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT3608 boost DCDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8Pcs DC-DC Adjustable Boost Module 2A DC Voltage Regulator Boost Plate Step Up Converter Module with USB 2V-24V to 5V 9V 12V 28V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B09ZKKFHXW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery holder w/leads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QTEATAK 4 x 1.5V AA Batteries Battery Holder Wire Leads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B085VS14TY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jumpers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUSTOR 560 Pieces Jumper Wire Kit 14 Lengths Assorted Preformed Breadboard Jumper Wire with Free Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07CJYSL2T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/M jumper cables long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDGELEC 120pcs 20cm Dupont Wire Male to Female Breadboard Jumper Wires 7.9 inch 1pin-1pin 2.54mm Connector for DIY Arduino Raspberry PI 10 15 20 30 40 50 100cm Optional Multicolored Ribbon Cables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07GD1TFBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/M jumper cables short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDGELEC 120pcs 10cm Dupont Wire Male to Female Breadboard Jumper Wires 3.9 inch 1pin-1pin 2.54mm Connector for DIY Arduino Raspberry PI 10 15 20 30 40 50 100cm Optional Multicolored Ribbon Cables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07GD1R5MS</t>
+  </si>
+  <si>
     <t xml:space="preserve">M2 / 10mm</t>
   </si>
   <si>
@@ -62,31 +125,79 @@
     <t xml:space="preserve">(same set)</t>
   </si>
   <si>
-    <t xml:space="preserve">small breadboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEYUE breadboard Set Prototype Board - 6 PCS 400 Pin Solderless Board Kit for Raspberry pi and Arduino Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07LFD4LT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#61 rubber band</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alliance Rubber 54615 Advantage Rubber Bands Size #61, 1 lb Box Contains Approx. 535 Bands (2inch x 1/4inch, Blue)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B008X09UNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT3608 boost DCDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8Pcs DC-DC Adjustable Boost Module 2A DC Voltage Regulator Boost Plate Step Up Converter Module with USB 2V-24V to 5V 9V 12V 28V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B09ZKKFHXW</t>
+    <t xml:space="preserve">M2 Nuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flyback diode 4004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOJACK 1N4004 Rectifier Diode 1 A 400 V DO-41 Axial 4004 1 amp 400 Volt Electronic Silicon Diodes(Pack of 125 Pieces)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07Q4F4RPZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resistors for LEDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDGELEC 100pcs 220 ohm Resistor 1/2w (0.5Watt) ±1% Tolerance Metal Film Fixed Resistor, Multiple Values of Resistance Optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07QK9ZBVZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M2 hex wrench</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tsnamay 2mm Hex Key Wrench L Shaped Hexagon Head Repairing Tool 50pcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B09R98WLZ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOJACK 5 Colors 500 pcs 5mm LED Diode Lights Assored Kit Pack Bright Lighting Bulb Lamps Electronics Components 5 mm Light Emitting Diodes Parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B09XDMJ6KY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BJT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCIGICM (200 Pcs) 2N2222 Transistor, 2N2222A to-92 Transistor NPN 40V 600mA 300MHz 625mW Through Hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B06XPWS52G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L293D motor controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridgold 10pcs L293 L293D 16-pin IC Stepper Motor Drivers Controllers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07NXTWJV9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pack of 25 Pieces) MCIGICM 74HC595 74595 SN74HC595N 8-Bit Shift Register DIP-16 IC 74hc595 Shift registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B07HFWB9L9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esp32cam with CH340C usb card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DORHEA 4 Set ESP32 Cam WiFi Bluetooth Development Board with OV2640 Camera Module + Micro USB to Serial Port CH340C 4.75V-5.25V Nodemcu for Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B09265G5Z4</t>
   </si>
   <si>
     <t xml:space="preserve">geared dc N20 motor</t>
@@ -107,49 +218,16 @@
     <t xml:space="preserve">https://www.amazon.com/dp/B072V529YD</t>
   </si>
   <si>
-    <t xml:space="preserve">L293D motor controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridgold 10pcs L293 L293D 16-pin IC Stepper Motor Drivers Controllers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07NXTWJV9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flyback diode 4004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOJACK 1N4004 Rectifier Diode 1 A 400 V DO-41 Axial 4004 1 amp 400 Volt Electronic Silicon Diodes(Pack of 125 Pieces)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07Q4F4RPZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEDs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOJACK 5 Colors 500 pcs 5mm LED Diode Lights Assored Kit Pack Bright Lighting Bulb Lamps Electronics Components 5 mm Light Emitting Diodes Parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B09XDMJ6KY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resistors for LEDs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDGELEC 100pcs 220 ohm Resistor 1/2w (0.5Watt) ±1% Tolerance Metal Film Fixed Resistor, Multiple Values of Resistance Optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07QK9ZBVZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BJT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCIGICM (200 Pcs) 2N2222 Transistor, 2N2222A to-92 Transistor NPN 40V 600mA 300MHz 625mW Through Hole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B06XPWS52G</t>
+    <t xml:space="preserve">pack of servo horns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cut to 2pc 88mm rods for axles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP-VIGOR 20pcs 2mm x 300mm Stainless Steel Rods for DIY Crafts, Metal Solid Round Shaft Rods Lathe Bar Stock for DIY Car Helicopter Airplane Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com//dp/B09WDCDCR6</t>
   </si>
   <si>
     <t xml:space="preserve">PLA</t>
@@ -161,78 +239,6 @@
     <t xml:space="preserve">https://www.amazon.com/dp/B085DX3X8Y</t>
   </si>
   <si>
-    <t xml:space="preserve">jumpers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUSTOR 560 Pieces Jumper Wire Kit 14 Lengths Assorted Preformed Breadboard Jumper Wire with Free Box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07CJYSL2T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">esp32cam with CH340C usb card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DORHEA 4 Set ESP32 Cam WiFi Bluetooth Development Board with OV2640 Camera Module + Micro USB to Serial Port CH340C 4.75V-5.25V Nodemcu for Raspberry Pi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B09265G5Z4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cut to 2pc 88mm rods for axles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOP-VIGOR 20pcs 2mm x 300mm Stainless Steel Rods for DIY Crafts, Metal Solid Round Shaft Rods Lathe Bar Stock for DIY Car Helicopter Airplane Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com//dp/B09WDCDCR6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">battery holder w/leads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QTEATAK 4 x 1.5V AA Batteries Battery Holder Wire Leads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B085VS14TY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M2 hex wrench</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tsnamay 2mm Hex Key Wrench L Shaped Hexagon Head Repairing Tool 50pcs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B09R98WLZ2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F/M jumper cables long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDGELEC 120pcs 20cm Dupont Wire Male to Female Breadboard Jumper Wires 7.9 inch 1pin-1pin 2.54mm Connector for DIY Arduino Raspberry PI 10 15 20 30 40 50 100cm Optional Multicolored Ribbon Cables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07GD1TFBR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F/M jumper cables short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDGELEC 120pcs 10cm Dupont Wire Male to Female Breadboard Jumper Wires 3.9 inch 1pin-1pin 2.54mm Connector for DIY Arduino Raspberry PI 10 15 20 30 40 50 100cm Optional Multicolored Ribbon Cables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07GD1R5MS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shift register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pack of 25 Pieces) MCIGICM 74HC595 74595 SN74HC595N 8-Bit Shift Register DIP-16 IC 74hc595 Shift registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B07HFWB9L9</t>
-  </si>
-  <si>
     <t xml:space="preserve">subtotal with USB programmer</t>
   </si>
   <si>
@@ -272,6 +278,9 @@
     <t xml:space="preserve">https://www.amazon.com/dp/B07KH8BG1F</t>
   </si>
   <si>
+    <t xml:space="preserve">only really need the flat one</t>
+  </si>
+  <si>
     <t xml:space="preserve">AA batteries</t>
   </si>
   <si>
@@ -281,7 +290,7 @@
     <t xml:space="preserve">https://www.amazon.com/dp/B01B8R6PF2</t>
   </si>
   <si>
-    <t xml:space="preserve">only really need the flat one</t>
+    <t xml:space="preserve">push buttons</t>
   </si>
   <si>
     <t xml:space="preserve">qty</t>
@@ -474,10 +483,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,23 +535,23 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11.99</v>
+        <v>7.99</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>140</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2" t="n">
-        <f aca="false">E2/F2</f>
-        <v>0.0856428571428572</v>
+        <f aca="false">E2/F2*A11</f>
+        <v>1.33166666666667</v>
       </c>
       <c r="H2" s="2" t="n">
         <f aca="false">G2*A2</f>
-        <v>0.0856428571428572</v>
+        <v>1.33166666666667</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>11</v>
@@ -550,13 +559,22 @@
       <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>535</v>
+      </c>
       <c r="G3" s="2" t="n">
-        <f aca="false">G2</f>
-        <v>0.0856428571428572</v>
+        <f aca="false">E3/F3</f>
+        <v>0.0141682242990654</v>
       </c>
       <c r="H3" s="2" t="n">
         <f aca="false">G3*A3</f>
-        <v>0.171285714285714</v>
+        <v>0.0566728971962617</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,223 +582,177 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>7.99</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2" t="n">
-        <f aca="false">E4/F4*A2</f>
-        <v>1.33166666666667</v>
+        <f aca="false">E4/F4</f>
+        <v>0.99875</v>
       </c>
       <c r="H4" s="2" t="n">
         <f aca="false">G4*A4</f>
-        <v>1.33166666666667</v>
+        <v>0.99875</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>7.58</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>535</v>
       </c>
       <c r="G5" s="2" t="n">
         <f aca="false">E5/F5</f>
-        <v>0.0141682242990654</v>
+        <v>1.7475</v>
       </c>
       <c r="H5" s="2" t="n">
         <f aca="false">G5*A5</f>
-        <v>0.0566728971962617</v>
+        <v>1.7475</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>7.99</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <f aca="false">E6/F6</f>
-        <v>0.99875</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <f aca="false">G6*A6</f>
-        <v>0.99875</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="2" t="n">
-        <v>9.99</v>
+        <v>11.99</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>3</v>
+        <v>560</v>
       </c>
       <c r="G7" s="2" t="n">
         <f aca="false">E7/F7</f>
-        <v>3.33</v>
+        <v>0.0214107142857143</v>
       </c>
       <c r="H7" s="2" t="n">
         <f aca="false">G7*A7</f>
-        <v>3.33</v>
+        <v>0.428214285714286</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" s="2" t="n">
-        <v>18.88</v>
+        <v>7.98</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="n">
         <f aca="false">E8/F8</f>
-        <v>1.888</v>
+        <v>0.0665</v>
       </c>
       <c r="H8" s="2" t="n">
         <f aca="false">G8*A8</f>
-        <v>1.888</v>
+        <v>0.665</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="E9" s="2" t="n">
-        <v>8.99</v>
+        <v>6.98</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">E9/F9</f>
-        <v>0.899</v>
+        <v>0.0581666666666667</v>
       </c>
       <c r="H9" s="2" t="n">
         <f aca="false">G9*A9</f>
-        <v>0.899</v>
+        <v>0.581666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>5.99</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>125</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <f aca="false">E10/F10</f>
-        <v>0.04792</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <f aca="false">G10*A10</f>
-        <v>0.04792</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>11.99</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>500</v>
+        <v>140</v>
       </c>
       <c r="G11" s="2" t="n">
         <f aca="false">E11/F11</f>
-        <v>0.02398</v>
+        <v>0.0856428571428572</v>
       </c>
       <c r="H11" s="2" t="n">
         <f aca="false">G11*A11</f>
-        <v>0.09592</v>
+        <v>0.0856428571428572</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,143 +760,144 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>5.99</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2" t="n">
-        <f aca="false">E12/F12</f>
-        <v>0.0599</v>
+        <f aca="false">G11</f>
+        <v>0.0856428571428572</v>
       </c>
       <c r="H12" s="2" t="n">
         <f aca="false">G12*A12</f>
-        <v>0.1198</v>
+        <v>0.171285714285714</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>6.99</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <f aca="false">E13/F13</f>
-        <v>0.03495</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <f aca="false">G13*A13</f>
-        <v>0.03495</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>36.99</v>
+        <v>5.99</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2000</v>
+        <v>125</v>
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">E14/F14</f>
-        <v>0.018495</v>
+        <v>0.04792</v>
       </c>
       <c r="H14" s="2" t="n">
         <f aca="false">G14*A14</f>
-        <v>0.88776</v>
+        <v>0.04792</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="A15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <f aca="false">E15/F15</f>
+        <v>0.0599</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <f aca="false">G15*A15</f>
+        <v>0.2396</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>11.99</v>
+        <v>6.99</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>560</v>
+        <v>50</v>
       </c>
       <c r="G16" s="2" t="n">
         <f aca="false">E16/F16</f>
-        <v>0.0214107142857143</v>
+        <v>0.1398</v>
       </c>
       <c r="H16" s="2" t="n">
         <f aca="false">G16*A16</f>
-        <v>0.428214285714286</v>
+        <v>0.1398</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>28.99</v>
+        <v>11.99</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>4</v>
+        <v>500</v>
       </c>
       <c r="G17" s="2" t="n">
         <f aca="false">E17/F17</f>
-        <v>7.2475</v>
+        <v>0.02398</v>
       </c>
       <c r="H17" s="2" t="n">
         <f aca="false">G17*A17</f>
-        <v>7.2475</v>
+        <v>0.09592</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,139 +905,88 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>9.59</v>
+        <v>6.99</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="G18" s="2" t="n">
         <f aca="false">E18/F18</f>
-        <v>0.4795</v>
+        <v>0.03495</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">G18*A18</f>
-        <v>0.4795</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>6.99</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <f aca="false">E19/F19</f>
-        <v>1.7475</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <f aca="false">G19*A19</f>
-        <v>1.7475</v>
+        <v>0.03495</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>6.99</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <f aca="false">E20/F20</f>
-        <v>0.1398</v>
-      </c>
-      <c r="H20" s="2" t="n">
-        <f aca="false">G20*A20</f>
-        <v>0.1398</v>
-      </c>
+      <c r="E20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>7.98</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>120</v>
       </c>
       <c r="G21" s="2" t="n">
         <f aca="false">E21/F21</f>
-        <v>0.0665</v>
+        <v>0.899</v>
       </c>
       <c r="H21" s="2" t="n">
         <f aca="false">G21*A21</f>
-        <v>0.665</v>
+        <v>0.899</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>6.98</v>
+        <v>6.99</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="G22" s="2" t="n">
         <f aca="false">E22/F22</f>
-        <v>0.0581666666666667</v>
+        <v>0.2796</v>
       </c>
       <c r="H22" s="2" t="n">
         <f aca="false">G22*A22</f>
-        <v>0.581666666666667</v>
+        <v>0.2796</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,224 +994,358 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>6.99</v>
+        <v>28.99</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G23" s="2" t="n">
         <f aca="false">E23/F23</f>
-        <v>0.2796</v>
+        <v>7.2475</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">G23*A23</f>
-        <v>0.2796</v>
-      </c>
+        <v>7.2475</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
-        <v>70</v>
+      <c r="A25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="E25" s="2" t="n">
-        <f aca="false">SUM(E2:E23)</f>
-        <v>227.86</v>
+        <v>9.99</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <f aca="false">E25/F25</f>
+        <v>3.33</v>
       </c>
       <c r="H25" s="2" t="n">
-        <f aca="false">SUM(H2:H23)</f>
-        <v>21.5161490876725</v>
+        <f aca="false">G25*A25</f>
+        <v>3.33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="A26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>18.88</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <f aca="false">E26/F26</f>
+        <v>1.888</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <f aca="false">G26*A26</f>
+        <v>1.888</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>9.59</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <f aca="false">E29/F29</f>
+        <v>0.4795</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <f aca="false">G29*A29</f>
+        <v>0.4795</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>36.99</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <f aca="false">E30/F30</f>
+        <v>0.018495</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <f aca="false">G30*A30</f>
+        <v>0.88776</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <f aca="false">SUM(E2:E30)</f>
+        <v>227.86</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <f aca="false">SUM(H2:H30)</f>
+        <v>21.6359490876725</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
         <v>-1</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="2" t="n">
+      <c r="B34" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="2" t="n">
         <v>28.99</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F34" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <f aca="false">E27/F27</f>
+      <c r="G34" s="2" t="n">
+        <f aca="false">E34/F34</f>
         <v>7.2475</v>
       </c>
-      <c r="H27" s="2" t="n">
-        <f aca="false">G27*A27</f>
+      <c r="H34" s="2" t="n">
+        <f aca="false">G34*A34</f>
         <v>-7.2475</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>24.99</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G28" s="2" t="n">
-        <f aca="false">E28/F28</f>
-        <v>6.2475</v>
-      </c>
-      <c r="H28" s="2" t="n">
-        <f aca="false">G28*A28</f>
-        <v>6.2475</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" s="2" t="n">
-        <f aca="false">SUM(H2:H23)+SUM(H27:H28)</f>
-        <v>20.5161490876725</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>17.16</v>
+        <v>24.99</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G35" s="2" t="n">
         <f aca="false">E35/F35</f>
-        <v>2.86</v>
+        <v>6.2475</v>
       </c>
       <c r="H35" s="2" t="n">
         <f aca="false">G35*A35</f>
+        <v>6.2475</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <f aca="false">SUM(H2:H30)+SUM(H34:H35)</f>
+        <v>20.6359490876725</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>17.16</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <f aca="false">E42/F42</f>
+        <v>2.86</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <f aca="false">G42*A42</f>
         <v>0.143</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="0" t="s">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="C43" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="2" t="n">
         <v>5.99</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F43" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G36" s="2" t="n">
-        <f aca="false">E36/F36</f>
+      <c r="G43" s="2" t="n">
+        <f aca="false">E43/F43</f>
         <v>0.998333333333333</v>
       </c>
-      <c r="H36" s="2" t="n">
-        <f aca="false">G36*A36</f>
+      <c r="H43" s="2" t="n">
+        <f aca="false">G43*A43</f>
         <v>0.998333333333333</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="I43" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="2" t="n">
+      <c r="B44" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="2" t="n">
         <v>25.76</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F44" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="G37" s="2" t="n">
-        <f aca="false">E37/F37</f>
+      <c r="G44" s="2" t="n">
+        <f aca="false">E44/F44</f>
         <v>0.2576</v>
       </c>
-      <c r="H37" s="2" t="n">
-        <f aca="false">G37*A37</f>
+      <c r="H44" s="2" t="n">
+        <f aca="false">G44*A44</f>
         <v>1.0304</v>
       </c>
-      <c r="I37" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1309,7 +1365,7 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -1325,22 +1381,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,10 +1404,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">3*60+15</f>
@@ -1369,10 +1425,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>16</v>
@@ -1389,10 +1445,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">3*60+7</f>
@@ -1410,10 +1466,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>24</v>
@@ -1430,10 +1486,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">2*60+13</f>
@@ -1446,7 +1502,7 @@
         <v>4.43</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1457,10 +1513,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>6</v>
@@ -1472,16 +1528,16 @@
         <v>0.13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,7 +1560,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(I8,"hrs", K8, "min")</f>

</xml_diff>